<commit_message>
backplane: add MFN & notes to BOM
</commit_message>
<xml_diff>
--- a/hardware/backplane/rev_c/backplane_bom.xlsx
+++ b/hardware/backplane/rev_c/backplane_bom.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19680" tabRatio="500"/>
+    <workbookView xWindow="14780" yWindow="460" windowWidth="18820" windowHeight="19660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="backplane_bom" localSheetId="0">Sheet1!$A$1:$J$31</definedName>
+    <definedName name="backplane_bom" localSheetId="0">Sheet1!$A$1:$O$31</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="211">
   <si>
     <t>Qty</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Package</t>
   </si>
   <si>
-    <t>Parts</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -475,13 +472,226 @@
   </si>
   <si>
     <t>DNP</t>
+  </si>
+  <si>
+    <t>Part Reference</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>8-TSSOP</t>
+  </si>
+  <si>
+    <t>Manufactuerer Part Number</t>
+  </si>
+  <si>
+    <t>Manufactuerer</t>
+  </si>
+  <si>
+    <t>SN75240PWR</t>
+  </si>
+  <si>
+    <t>SFH11-PBPC-D07-ST-BK</t>
+  </si>
+  <si>
+    <t>Sullins Connector</t>
+  </si>
+  <si>
+    <t>PTH 14 pins</t>
+  </si>
+  <si>
+    <t>**2 Parts** PTH 20 pins + PTH 10 pins</t>
+  </si>
+  <si>
+    <t>SFH11-PBPC-D10-ST-BK</t>
+  </si>
+  <si>
+    <t>SFH11-PBPC-D10-ST-BK and SFH11-PBPC-D05-ST-BK</t>
+  </si>
+  <si>
+    <t>Do Not Insert</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Must be 5% or better</t>
+  </si>
+  <si>
+    <t>CL10C220JB8NNNC</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>GRM1555C1H220JA01D</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM188R71E104KA01D</t>
+  </si>
+  <si>
+    <t>CL32A157MQVNNNE</t>
+  </si>
+  <si>
+    <t>GRM31CR60J157ME11L</t>
+  </si>
+  <si>
+    <t>Can Substitue?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Note: Any part marked "Can Substitue" can be substituted for any equal size/value parts</t>
+  </si>
+  <si>
+    <t>PTH 20 pins</t>
+  </si>
+  <si>
+    <t>PTH 2 pins</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>MCR01MRTJ270</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>MCR03ERTF49R9</t>
+  </si>
+  <si>
+    <t>MCR03EZPFX1501</t>
+  </si>
+  <si>
+    <t>MCR03EZPFX1002</t>
+  </si>
+  <si>
+    <t>MCR03ERTF1502</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ106</t>
+  </si>
+  <si>
+    <t>SIP32402ADNP-T1GE4</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>4-UFDFN Exposed Pad</t>
+  </si>
+  <si>
+    <t>8-TSSOP Exposed Pad</t>
+  </si>
+  <si>
+    <t>AP2401MP-13</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>6-TSSOP</t>
+  </si>
+  <si>
+    <t>NC7SZ157P6X</t>
+  </si>
+  <si>
+    <t>Fairchild/ON Semiconductor</t>
+  </si>
+  <si>
+    <t>PTH 1 pin</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>48-LQFP</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>8-UFQFN</t>
+  </si>
+  <si>
+    <t>FXMA2102UMX</t>
+  </si>
+  <si>
+    <t>10-UFQFN</t>
+  </si>
+  <si>
+    <t>TS3USB30ERSWR</t>
+  </si>
+  <si>
+    <t>20-VFQFN Exposed Pad</t>
+  </si>
+  <si>
+    <t>MCP23008-E/ML</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>5-TSOP</t>
+  </si>
+  <si>
+    <t>NCP301LSN30T1G</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>Power-on-Reset with Open Collector output - 2.9-3.1V threshold okay</t>
+  </si>
+  <si>
+    <t>8-SOIC</t>
+  </si>
+  <si>
+    <t>M24C01-WMN6TP</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>8-VFSOP</t>
+  </si>
+  <si>
+    <t>SN74LVC2T45DCUR</t>
+  </si>
+  <si>
+    <t>ABMM-6.000MHZ-B2-T</t>
+  </si>
+  <si>
+    <t>Abracon LLC</t>
+  </si>
+  <si>
+    <t>J3 is two physical parts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -497,16 +707,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -514,19 +758,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC6EFCE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -802,664 +1124,1060 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="O1" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="O2" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" t="s">
         <v>130</v>
       </c>
-      <c r="F3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" t="s">
+        <v>158</v>
+      </c>
+      <c r="K5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" t="s">
         <v>112</v>
       </c>
-      <c r="C7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="J7" t="s">
+        <v>191</v>
+      </c>
+      <c r="K7" t="s">
         <v>113</v>
       </c>
-      <c r="F7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
+        <v>149</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J8" t="s">
+        <v>148</v>
+      </c>
+      <c r="K8" t="s">
         <v>59</v>
       </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F9" t="s">
+      <c r="L9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="O9" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>169</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" t="s">
         <v>95</v>
       </c>
-      <c r="C11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1725656</v>
+      </c>
+      <c r="J11" t="s">
+        <v>171</v>
+      </c>
+      <c r="K11" t="s">
         <v>96</v>
       </c>
-      <c r="F11" t="s">
+      <c r="M11" t="s">
         <v>97</v>
       </c>
-      <c r="H11" t="s">
+      <c r="N11" t="s">
         <v>98</v>
       </c>
-      <c r="I11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
         <v>71</v>
       </c>
-      <c r="C12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>142</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" t="s">
+        <v>173</v>
+      </c>
+      <c r="K13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J14" t="s">
+        <v>173</v>
+      </c>
+      <c r="K14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="J15" t="s">
+        <v>173</v>
+      </c>
+      <c r="K15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J16" t="s">
+        <v>173</v>
+      </c>
+      <c r="K16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="J17" t="s">
+        <v>173</v>
+      </c>
+      <c r="K17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="J18" t="s">
+        <v>173</v>
+      </c>
+      <c r="K18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>27</v>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>139</v>
       </c>
       <c r="F19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" t="s">
         <v>102</v>
       </c>
-      <c r="C20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
+        <v>181</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="J20" t="s">
+        <v>180</v>
+      </c>
+      <c r="K20" t="s">
         <v>103</v>
       </c>
-      <c r="F20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
+        <v>182</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="J21" t="s">
+        <v>184</v>
+      </c>
+      <c r="K21" t="s">
         <v>48</v>
       </c>
-      <c r="F21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="H22" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="J22" t="s">
+        <v>187</v>
+      </c>
+      <c r="K22" t="s">
         <v>86</v>
       </c>
-      <c r="F22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" t="s">
         <v>117</v>
       </c>
-      <c r="C23" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
+        <v>188</v>
+      </c>
+      <c r="I23" s="9">
+        <v>5001</v>
+      </c>
+      <c r="J23" t="s">
+        <v>189</v>
+      </c>
+      <c r="K23" t="s">
         <v>118</v>
       </c>
-      <c r="F23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" t="s">
+        <v>166</v>
+      </c>
+      <c r="E24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" t="s">
         <v>127</v>
       </c>
-      <c r="C24" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I24" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>191</v>
+      </c>
+      <c r="K24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" t="s">
         <v>67</v>
       </c>
-      <c r="C25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
+        <v>192</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="J25" t="s">
+        <v>187</v>
+      </c>
+      <c r="K25" t="s">
         <v>68</v>
       </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" t="s">
         <v>122</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="H26" t="s">
+        <v>194</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="J26" t="s">
+        <v>191</v>
+      </c>
+      <c r="K26" t="s">
         <v>123</v>
       </c>
-      <c r="F26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" t="s">
         <v>80</v>
       </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="H27" t="s">
+        <v>196</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="J27" t="s">
+        <v>198</v>
+      </c>
+      <c r="K27" t="s">
         <v>81</v>
       </c>
-      <c r="F27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
         <v>90</v>
       </c>
-      <c r="C28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="H28" t="s">
+        <v>199</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="J28" t="s">
+        <v>201</v>
+      </c>
+      <c r="K28" t="s">
         <v>91</v>
       </c>
-      <c r="F28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="O28" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" t="s">
         <v>75</v>
       </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="H29" t="s">
+        <v>203</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J29" t="s">
+        <v>205</v>
+      </c>
+      <c r="K29" t="s">
         <v>76</v>
       </c>
-      <c r="F29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" t="s">
         <v>107</v>
       </c>
-      <c r="C30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="H30" t="s">
+        <v>206</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="J30" t="s">
+        <v>191</v>
+      </c>
+      <c r="K30" t="s">
         <v>108</v>
       </c>
-      <c r="F30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" t="s">
         <v>42</v>
       </c>
-      <c r="C31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="H31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J31" t="s">
+        <v>209</v>
+      </c>
+      <c r="K31" t="s">
         <v>43</v>
       </c>
-      <c r="F31" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B34:F34"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D2:D31">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
backplane: fix 4.7 uF part number in BOM
</commit_message>
<xml_diff>
--- a/hardware/backplane/rev_c/backplane_bom.xlsx
+++ b/hardware/backplane/rev_c/backplane_bom.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="460" windowWidth="18820" windowHeight="19660" tabRatio="500"/>
+    <workbookView xWindow="5240" yWindow="460" windowWidth="31780" windowHeight="19660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,9 +450,6 @@
     <t>490-1524-1-ND</t>
   </si>
   <si>
-    <t>1276-3367-1-ND</t>
-  </si>
-  <si>
     <t>RHM27CECT-ND</t>
   </si>
   <si>
@@ -486,12 +483,6 @@
     <t>8-TSSOP</t>
   </si>
   <si>
-    <t>Manufactuerer Part Number</t>
-  </si>
-  <si>
-    <t>Manufactuerer</t>
-  </si>
-  <si>
     <t>SN75240PWR</t>
   </si>
   <si>
@@ -540,9 +531,6 @@
     <t>GRM188R71E104KA01D</t>
   </si>
   <si>
-    <t>CL32A157MQVNNNE</t>
-  </si>
-  <si>
     <t>GRM31CR60J157ME11L</t>
   </si>
   <si>
@@ -685,6 +673,18 @@
   </si>
   <si>
     <t>J3 is two physical parts</t>
+  </si>
+  <si>
+    <t>1276-2087-2-ND</t>
+  </si>
+  <si>
+    <t>CL10B475KQ8NQNC</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
   </si>
 </sst>
 </file>
@@ -793,7 +793,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -807,9 +807,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -825,6 +822,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1126,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1139,7 @@
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
     <col min="7" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="9" customWidth="1"/>
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
     <col min="11" max="11" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -1152,13 +1153,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -1170,13 +1171,13 @@
         <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>209</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>4</v>
@@ -1191,7 +1192,7 @@
         <v>7</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1202,7 +1203,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
@@ -1214,19 +1215,19 @@
         <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>157</v>
+        <v>141</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>154</v>
       </c>
       <c r="J2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K2" t="s">
         <v>32</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1237,7 +1238,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -1249,13 +1250,13 @@
         <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>159</v>
+        <v>141</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="J3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K3" t="s">
         <v>130</v>
@@ -1269,7 +1270,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -1281,13 +1282,13 @@
         <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>161</v>
+        <v>141</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="J4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K4" t="s">
         <v>131</v>
@@ -1301,7 +1302,7 @@
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -1313,16 +1314,16 @@
         <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>162</v>
+        <v>141</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="J5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K5" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1333,7 +1334,7 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1345,13 +1346,13 @@
         <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>163</v>
+        <v>141</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="J6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K6" t="s">
         <v>23</v>
@@ -1365,7 +1366,7 @@
         <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
         <v>109</v>
@@ -1377,13 +1378,13 @@
         <v>112</v>
       </c>
       <c r="H7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>146</v>
-      </c>
       <c r="J7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K7" t="s">
         <v>113</v>
@@ -1397,7 +1398,7 @@
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
@@ -1409,13 +1410,13 @@
         <v>58</v>
       </c>
       <c r="H8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="J8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K8" t="s">
         <v>59</v>
@@ -1429,7 +1430,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>49</v>
@@ -1441,13 +1442,13 @@
         <v>52</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>53</v>
@@ -1456,7 +1457,7 @@
         <v>54</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -1467,7 +1468,7 @@
         <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E10" t="s">
         <v>60</v>
@@ -1479,13 +1480,13 @@
         <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>169</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>151</v>
+        <v>165</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="J10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K10" t="s">
         <v>53</v>
@@ -1499,7 +1500,7 @@
         <v>94</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E11" t="s">
         <v>92</v>
@@ -1511,13 +1512,13 @@
         <v>95</v>
       </c>
       <c r="H11" t="s">
-        <v>170</v>
-      </c>
-      <c r="I11" s="9">
+        <v>166</v>
+      </c>
+      <c r="I11" s="8">
         <v>1725656</v>
       </c>
       <c r="J11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K11" t="s">
         <v>96</v>
@@ -1537,13 +1538,13 @@
         <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" t="s">
         <v>69</v>
@@ -1552,7 +1553,7 @@
         <v>71</v>
       </c>
       <c r="K12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1563,7 +1564,7 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1575,16 +1576,16 @@
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>142</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>172</v>
+        <v>141</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="J13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1595,7 +1596,7 @@
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
@@ -1607,16 +1608,16 @@
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>142</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>174</v>
+        <v>141</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="J14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1627,7 +1628,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1639,16 +1640,16 @@
         <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>142</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>175</v>
+        <v>141</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="J15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="32" x14ac:dyDescent="0.2">
@@ -1659,7 +1660,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
@@ -1671,16 +1672,16 @@
         <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>142</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>176</v>
+        <v>141</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="J16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -1691,7 +1692,7 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -1703,16 +1704,16 @@
         <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>142</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>177</v>
+        <v>141</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="J17" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
@@ -1723,7 +1724,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -1735,16 +1736,16 @@
         <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>142</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>178</v>
+        <v>141</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="J18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
@@ -1755,13 +1756,13 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
@@ -1770,7 +1771,7 @@
         <v>11</v>
       </c>
       <c r="K19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1781,7 +1782,7 @@
         <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
         <v>99</v>
@@ -1793,13 +1794,13 @@
         <v>102</v>
       </c>
       <c r="H20" t="s">
-        <v>181</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="J20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K20" t="s">
         <v>103</v>
@@ -1813,7 +1814,7 @@
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
@@ -1825,13 +1826,13 @@
         <v>47</v>
       </c>
       <c r="H21" t="s">
-        <v>182</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="J21" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K21" t="s">
         <v>48</v>
@@ -1845,7 +1846,7 @@
         <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E22" t="s">
         <v>82</v>
@@ -1857,13 +1858,13 @@
         <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>185</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="J22" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K22" t="s">
         <v>86</v>
@@ -1877,7 +1878,7 @@
         <v>116</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E23" t="s">
         <v>114</v>
@@ -1889,13 +1890,13 @@
         <v>117</v>
       </c>
       <c r="H23" t="s">
-        <v>188</v>
-      </c>
-      <c r="I23" s="9">
+        <v>184</v>
+      </c>
+      <c r="I23" s="8">
         <v>5001</v>
       </c>
       <c r="J23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K23" t="s">
         <v>118</v>
@@ -1909,7 +1910,7 @@
         <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E24" t="s">
         <v>124</v>
@@ -1921,13 +1922,13 @@
         <v>127</v>
       </c>
       <c r="H24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I24" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="I24" s="11" t="s">
         <v>128</v>
       </c>
       <c r="J24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K24" t="s">
         <v>128</v>
@@ -1941,7 +1942,7 @@
         <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E25" t="s">
         <v>64</v>
@@ -1953,13 +1954,13 @@
         <v>67</v>
       </c>
       <c r="H25" t="s">
-        <v>192</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>193</v>
+        <v>188</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="J25" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K25" t="s">
         <v>68</v>
@@ -1973,7 +1974,7 @@
         <v>121</v>
       </c>
       <c r="D26" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E26" t="s">
         <v>119</v>
@@ -1985,13 +1986,13 @@
         <v>122</v>
       </c>
       <c r="H26" t="s">
-        <v>194</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="J26" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K26" t="s">
         <v>123</v>
@@ -2005,7 +2006,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E27" t="s">
         <v>77</v>
@@ -2017,13 +2018,13 @@
         <v>80</v>
       </c>
       <c r="H27" t="s">
-        <v>196</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="J27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K27" t="s">
         <v>81</v>
@@ -2037,7 +2038,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E28" t="s">
         <v>87</v>
@@ -2049,19 +2050,19 @@
         <v>90</v>
       </c>
       <c r="H28" t="s">
-        <v>199</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>200</v>
+        <v>195</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>196</v>
       </c>
       <c r="J28" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K28" t="s">
         <v>91</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -2072,7 +2073,7 @@
         <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E29" t="s">
         <v>72</v>
@@ -2084,13 +2085,13 @@
         <v>75</v>
       </c>
       <c r="H29" t="s">
-        <v>203</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>204</v>
+        <v>199</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>200</v>
       </c>
       <c r="J29" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K29" t="s">
         <v>76</v>
@@ -2104,7 +2105,7 @@
         <v>106</v>
       </c>
       <c r="D30" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E30" t="s">
         <v>104</v>
@@ -2116,13 +2117,13 @@
         <v>107</v>
       </c>
       <c r="H30" t="s">
-        <v>206</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>207</v>
+        <v>202</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>203</v>
       </c>
       <c r="J30" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K30" t="s">
         <v>108</v>
@@ -2136,7 +2137,7 @@
         <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
         <v>40</v>
@@ -2148,26 +2149,26 @@
         <v>42</v>
       </c>
       <c r="H31" t="s">
-        <v>142</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>208</v>
+        <v>141</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>204</v>
       </c>
       <c r="J31" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K31" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="B34" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>